<commit_message>
Codigos coletaveis e troca de mapa ao coletar todos.
</commit_message>
<xml_diff>
--- a/Conteudo/Layouts do jogo.xlsx
+++ b/Conteudo/Layouts do jogo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianca\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schmi\Documents\GitHub\2021gamet4-bianca-e-alisson\Conteudo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E99A9B-ED10-4B15-9797-D6680EBA92F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C5EE17-EA5D-4FF5-B746-09EF5783D451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="6" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
   </bookViews>
   <sheets>
     <sheet name="map 1" sheetId="6" r:id="rId1"/>
@@ -2001,146 +2001,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>174625</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>117475</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="45" name="Retângulo: Cantos Arredondados 44">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BD566C9-12D7-40F9-8730-02A8601B08E2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3524250" y="6429375"/>
-          <a:ext cx="4943475" cy="482600"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="2400">
-              <a:solidFill>
-                <a:srgbClr val="480048"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Iniciar</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>168275</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>111125</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="Retângulo: Cantos Arredondados 45">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67729FFE-FF40-430F-A122-705AF3FCFFBF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3517900" y="6946900"/>
-          <a:ext cx="4943475" cy="482600"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="2400">
-              <a:solidFill>
-                <a:srgbClr val="480048"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Sair</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>301625</xdr:colOff>
       <xdr:row>53</xdr:row>
@@ -3288,6 +3148,206 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190687</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>109258</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>140260</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85165</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Agrupar 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4C73DEE-6E27-4DD8-88E8-33D95023F28F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3563658" y="6205258"/>
+          <a:ext cx="4992220" cy="1499907"/>
+          <a:chOff x="3541246" y="6429375"/>
+          <a:chExt cx="4992220" cy="1499907"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="45" name="Retângulo: Cantos Arredondados 44">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BD566C9-12D7-40F9-8730-02A8601B08E2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3547596" y="6429375"/>
+            <a:ext cx="4985497" cy="482600"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="2400">
+                <a:solidFill>
+                  <a:srgbClr val="480048"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>JOGAR</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="46" name="Retângulo: Cantos Arredondados 45">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67729FFE-FF40-430F-A122-705AF3FCFFBF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3541246" y="6946900"/>
+            <a:ext cx="4985497" cy="482600"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="2400">
+                <a:solidFill>
+                  <a:srgbClr val="480048"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>controles</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="49" name="Retângulo: Cantos Arredondados 48">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{092E0982-9D31-4BB1-B191-5466CC65E284}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3547969" y="7446682"/>
+            <a:ext cx="4985497" cy="482600"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="2400">
+                <a:solidFill>
+                  <a:srgbClr val="480048"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>sair</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9437,8 +9497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C148A10E-86B2-4F0D-89D7-C11619B1E705}">
   <dimension ref="A1:AM73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="BI69" sqref="BI69"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AU29" sqref="AU29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
atualização planilha de layouts
</commit_message>
<xml_diff>
--- a/Conteudo/Layouts do jogo.xlsx
+++ b/Conteudo/Layouts do jogo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianca\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianca\Documents\GitHub\2021gamet4-bianca-e-alisson\Conteudo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E99A9B-ED10-4B15-9797-D6680EBA92F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA2366-6574-4B25-A2A1-E436A581B564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
   </bookViews>
   <sheets>
     <sheet name="map 1" sheetId="6" r:id="rId1"/>
@@ -151,9 +151,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF762700"/>
       <color rgb="FF480048"/>
       <color rgb="FF660066"/>
-      <color rgb="FF762700"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3590,8 +3590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA10F6F-187F-403F-8EDB-C58B1D6FC71F}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9:T9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3967,8 +3967,8 @@
         <v>11</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="1"/>
@@ -4560,7 +4560,7 @@
   <dimension ref="A1:AP22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AH32" sqref="AH32"/>
+      <selection activeCell="C10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4947,8 +4947,8 @@
         <v>11</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="1"/>
@@ -9437,7 +9437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C148A10E-86B2-4F0D-89D7-C11619B1E705}">
   <dimension ref="A1:AM73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="BI69" sqref="BI69"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Revert "atualização planilha de layouts"
This reverts commit f5c29d2902aba77524d53d66c299b7f5957e8573.
</commit_message>
<xml_diff>
--- a/Conteudo/Layouts do jogo.xlsx
+++ b/Conteudo/Layouts do jogo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianca\Documents\GitHub\2021gamet4-bianca-e-alisson\Conteudo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianca\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CA2366-6574-4B25-A2A1-E436A581B564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E99A9B-ED10-4B15-9797-D6680EBA92F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
   </bookViews>
   <sheets>
     <sheet name="map 1" sheetId="6" r:id="rId1"/>
@@ -151,9 +151,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF762700"/>
       <color rgb="FF480048"/>
       <color rgb="FF660066"/>
+      <color rgb="FF762700"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3590,8 +3590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA10F6F-187F-403F-8EDB-C58B1D6FC71F}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D10"/>
+    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9:T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3967,8 +3967,8 @@
         <v>11</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="1"/>
@@ -4560,7 +4560,7 @@
   <dimension ref="A1:AP22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D10"/>
+      <selection activeCell="AH32" sqref="AH32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4947,8 +4947,8 @@
         <v>11</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="1"/>
@@ -9437,7 +9437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C148A10E-86B2-4F0D-89D7-C11619B1E705}">
   <dimension ref="A1:AM73"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="BI69" sqref="BI69"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ajuste do menu inicial
</commit_message>
<xml_diff>
--- a/Conteudo/Layouts do jogo.xlsx
+++ b/Conteudo/Layouts do jogo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianca\Documents\GitHub\2021gamet4-bianca-e-alisson\Conteudo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7729CDA3-0A75-44B3-997B-2AFA6794E9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9717F2B5-12CE-44C4-A340-B1A1BCBCA337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="7" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
   </bookViews>
   <sheets>
     <sheet name="map 1" sheetId="6" r:id="rId1"/>
@@ -56,7 +56,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +105,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -133,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -144,6 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,6 +159,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE7E6E6"/>
       <color rgb="FF762700"/>
       <color rgb="FF480048"/>
       <color rgb="FF660066"/>
@@ -8519,7 +8527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEEB372-9C09-4E52-86CA-99BF55B745CD}">
   <dimension ref="A1:AN22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="AL32" sqref="AL32"/>
     </sheetView>
   </sheetViews>
@@ -10467,8 +10475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C148A10E-86B2-4F0D-89D7-C11619B1E705}">
   <dimension ref="A1:AM73"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AU29" sqref="AU29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10744,7 +10752,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>

</xml_diff>

<commit_message>
ajuste da tela de próxima fase
</commit_message>
<xml_diff>
--- a/Conteudo/Layouts do jogo.xlsx
+++ b/Conteudo/Layouts do jogo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianca\Documents\GitHub\2021gamet4-bianca-e-alisson\Conteudo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9717F2B5-12CE-44C4-A340-B1A1BCBCA337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAA5C32-BB15-4AD9-AF87-8C36AC5E2999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="7" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
   </bookViews>
   <sheets>
     <sheet name="map 1" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>trabalho a ser pego</t>
   </si>
@@ -42,15 +42,43 @@
   <si>
     <t>deixa o aluno lento</t>
   </si>
+  <si>
+    <t>tempos</t>
+  </si>
+  <si>
+    <t>bianca - 01:08</t>
+  </si>
+  <si>
+    <t>bianca - 01:03</t>
+  </si>
+  <si>
+    <t>bianca - 01:009</t>
+  </si>
+  <si>
+    <t>bianca - 00:59</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -151,6 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4626,10 +4655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4664F8D6-9700-412C-9949-8B3F40F9E4BF}">
-  <dimension ref="A1:AP22"/>
+  <dimension ref="A1:BE32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AI3" sqref="AI3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4640,7 +4669,11 @@
     <col min="38" max="39" width="2.7109375" customWidth="1"/>
     <col min="40" max="40" width="1.5703125" customWidth="1"/>
     <col min="41" max="41" width="5.85546875" customWidth="1"/>
-    <col min="42" max="55" width="2.7109375" customWidth="1"/>
+    <col min="42" max="47" width="2.7109375" customWidth="1"/>
+    <col min="48" max="48" width="27.7109375" customWidth="1"/>
+    <col min="49" max="50" width="3.140625" customWidth="1"/>
+    <col min="51" max="55" width="2.7109375" customWidth="1"/>
+    <col min="57" max="57" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">
@@ -5295,7 +5328,7 @@
       <c r="AI16" s="6"/>
       <c r="AJ16" s="2"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -5335,7 +5368,7 @@
       <c r="AI17" s="2"/>
       <c r="AJ17" s="2"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -5375,7 +5408,7 @@
       <c r="AI18" s="1"/>
       <c r="AJ18" s="2"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -5415,7 +5448,7 @@
       <c r="AI19" s="1"/>
       <c r="AJ19" s="2"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -5455,7 +5488,7 @@
       <c r="AI20" s="3"/>
       <c r="AJ20" s="2"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -5495,7 +5528,7 @@
       <c r="AI21" s="2"/>
       <c r="AJ21" s="2"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0</v>
       </c>
@@ -5602,7 +5635,33 @@
         <v>34</v>
       </c>
     </row>
+    <row r="28" spans="1:57" ht="21" x14ac:dyDescent="0.35">
+      <c r="BE28" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:57" ht="21" x14ac:dyDescent="0.35">
+      <c r="BE29" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:57" ht="21" x14ac:dyDescent="0.35">
+      <c r="BE30" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:57" ht="21" x14ac:dyDescent="0.35">
+      <c r="BE31" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:57" ht="21" x14ac:dyDescent="0.35">
+      <c r="BE32" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10475,7 +10534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C148A10E-86B2-4F0D-89D7-C11619B1E705}">
   <dimension ref="A1:AM73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ajustes NexFaseScreen + criação LoseScreen + atualização de mapa
</commit_message>
<xml_diff>
--- a/Conteudo/Layouts do jogo.xlsx
+++ b/Conteudo/Layouts do jogo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bianca\Documents\GitHub\2021gamet4-bianca-e-alisson\Conteudo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAA5C32-BB15-4AD9-AF87-8C36AC5E2999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF8C2B8-0F9F-4E12-94D8-AC28094F7914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
+    <workbookView xWindow="2460" yWindow="1755" windowWidth="15375" windowHeight="8580" firstSheet="3" activeTab="5" xr2:uid="{0B142173-238F-4730-919D-A327EE70452F}"/>
   </bookViews>
   <sheets>
     <sheet name="map 1" sheetId="6" r:id="rId1"/>
@@ -188,8 +188,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF762700"/>
       <color rgb="FFE7E6E6"/>
-      <color rgb="FF762700"/>
       <color rgb="FF480048"/>
       <color rgb="FF660066"/>
     </mruColors>
@@ -4657,8 +4657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4664F8D6-9700-412C-9949-8B3F40F9E4BF}">
   <dimension ref="A1:BE32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5:Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6639,7 +6639,7 @@
   <dimension ref="A1:AN22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="AF18" sqref="AF18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6919,7 +6919,7 @@
       <c r="V7" s="6"/>
       <c r="W7" s="2"/>
       <c r="X7" s="1"/>
-      <c r="Y7" s="4"/>
+      <c r="Y7" s="1"/>
       <c r="Z7" s="4"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="2"/>
@@ -7114,7 +7114,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="4"/>
+      <c r="L12" s="1"/>
       <c r="M12" s="4"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -7430,8 +7430,8 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="4"/>
@@ -8586,8 +8586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEEB372-9C09-4E52-86CA-99BF55B745CD}">
   <dimension ref="A1:AN22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AL32" sqref="AL32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AH9" sqref="AH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>